<commit_message>
Add test write manufactory code
</commit_message>
<xml_diff>
--- a/MWM/TestApp_LastUpdate14030802/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp_LastUpdate14030802/_Files/Exel/MWM.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5717EA55-7955-4ED2-B0F0-BEAEB84906C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7785"/>
+    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestResult" sheetId="1" r:id="rId1"/>
@@ -4235,16 +4236,16 @@
     <t>E01703CDB35FA8BB5F91830942D88844</t>
   </si>
   <si>
-    <t>1403-04-03 10:07:07</t>
-  </si>
-  <si>
-    <t>ED89A2877EAC19DC3C72050150AB6D97</t>
+    <t>1403-08-06 09:34:29</t>
+  </si>
+  <si>
+    <t>27D44453BAAF4E6DE0A63E8CC43B97DC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4424,7 +4425,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="746">
+  <cellXfs count="747">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6624,6 +6625,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6633,12 +6646,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6646,9 +6653,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6932,7 +6936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU923"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A563" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -6972,238 +6976,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:99" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="737" t="s">
+      <c r="A1" s="741" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="742" t="s">
+      <c r="B1" s="744" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="743"/>
-      <c r="D1" s="743"/>
-      <c r="E1" s="743"/>
-      <c r="F1" s="743"/>
-      <c r="G1" s="743"/>
-      <c r="H1" s="743"/>
-      <c r="I1" s="743"/>
-      <c r="J1" s="743"/>
-      <c r="K1" s="743"/>
-      <c r="L1" s="743"/>
-      <c r="M1" s="743"/>
-      <c r="N1" s="743"/>
-      <c r="O1" s="743"/>
-      <c r="P1" s="743"/>
-      <c r="Q1" s="743"/>
-      <c r="R1" s="743"/>
-      <c r="S1" s="743"/>
-      <c r="T1" s="743"/>
-      <c r="U1" s="743"/>
-      <c r="V1" s="743"/>
-      <c r="W1" s="743"/>
-      <c r="X1" s="743"/>
-      <c r="Y1" s="743"/>
-      <c r="Z1" s="743"/>
-      <c r="AA1" s="743"/>
-      <c r="AB1" s="743"/>
-      <c r="AC1" s="743"/>
-      <c r="AD1" s="743"/>
-      <c r="AE1" s="743"/>
-      <c r="AF1" s="743"/>
-      <c r="AG1" s="744"/>
+      <c r="C1" s="745"/>
+      <c r="D1" s="745"/>
+      <c r="E1" s="745"/>
+      <c r="F1" s="745"/>
+      <c r="G1" s="745"/>
+      <c r="H1" s="745"/>
+      <c r="I1" s="745"/>
+      <c r="J1" s="745"/>
+      <c r="K1" s="745"/>
+      <c r="L1" s="745"/>
+      <c r="M1" s="745"/>
+      <c r="N1" s="745"/>
+      <c r="O1" s="745"/>
+      <c r="P1" s="745"/>
+      <c r="Q1" s="745"/>
+      <c r="R1" s="745"/>
+      <c r="S1" s="745"/>
+      <c r="T1" s="745"/>
+      <c r="U1" s="745"/>
+      <c r="V1" s="745"/>
+      <c r="W1" s="745"/>
+      <c r="X1" s="745"/>
+      <c r="Y1" s="745"/>
+      <c r="Z1" s="745"/>
+      <c r="AA1" s="745"/>
+      <c r="AB1" s="745"/>
+      <c r="AC1" s="745"/>
+      <c r="AD1" s="745"/>
+      <c r="AE1" s="745"/>
+      <c r="AF1" s="745"/>
+      <c r="AG1" s="746"/>
     </row>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A2" s="738"/>
-      <c r="B2" s="740" t="s">
+      <c r="A2" s="742"/>
+      <c r="B2" s="739" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="740" t="s">
+      <c r="C2" s="739" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="740" t="s">
+      <c r="D2" s="739" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="740" t="s">
+      <c r="E2" s="739" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="740" t="s">
+      <c r="F2" s="739" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="740" t="s">
+      <c r="G2" s="739" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="740" t="s">
+      <c r="H2" s="739" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="740" t="s">
+      <c r="I2" s="739" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="740" t="s">
+      <c r="J2" s="739" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="740" t="s">
+      <c r="K2" s="739" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="740" t="s">
+      <c r="L2" s="739" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="740" t="s">
+      <c r="M2" s="739" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="740" t="s">
+      <c r="N2" s="739" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="740" t="s">
+      <c r="O2" s="739" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="740" t="s">
+      <c r="P2" s="739" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="740" t="s">
+      <c r="Q2" s="739" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="740" t="s">
+      <c r="R2" s="739" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="740" t="s">
+      <c r="S2" s="739" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="740" t="s">
+      <c r="T2" s="739" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="740" t="s">
+      <c r="U2" s="739" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="740" t="s">
+      <c r="V2" s="739" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="740" t="s">
+      <c r="W2" s="739" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="740" t="s">
+      <c r="X2" s="739" t="s">
         <v>30</v>
       </c>
-      <c r="Y2" s="740" t="s">
+      <c r="Y2" s="739" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="740" t="s">
+      <c r="Z2" s="739" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="740" t="s">
+      <c r="AA2" s="739" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="740" t="s">
+      <c r="AB2" s="739" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="740" t="s">
+      <c r="AC2" s="739" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="740" t="s">
+      <c r="AD2" s="739" t="s">
         <v>6</v>
       </c>
-      <c r="AE2" s="740" t="s">
+      <c r="AE2" s="739" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="740" t="s">
+      <c r="AF2" s="739" t="s">
         <v>5</v>
       </c>
-      <c r="AG2" s="740" t="s">
+      <c r="AG2" s="739" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="739"/>
-      <c r="B3" s="741"/>
-      <c r="C3" s="741"/>
-      <c r="D3" s="741"/>
-      <c r="E3" s="741"/>
-      <c r="F3" s="741"/>
-      <c r="G3" s="741"/>
-      <c r="H3" s="741"/>
-      <c r="I3" s="741"/>
-      <c r="J3" s="741"/>
-      <c r="K3" s="741"/>
-      <c r="L3" s="741"/>
-      <c r="M3" s="741"/>
-      <c r="N3" s="741"/>
-      <c r="O3" s="741"/>
-      <c r="P3" s="741"/>
-      <c r="Q3" s="741"/>
-      <c r="R3" s="741"/>
-      <c r="S3" s="741"/>
-      <c r="T3" s="741"/>
-      <c r="U3" s="741"/>
-      <c r="V3" s="741"/>
-      <c r="W3" s="741"/>
-      <c r="X3" s="741"/>
-      <c r="Y3" s="741"/>
-      <c r="Z3" s="741"/>
-      <c r="AA3" s="741"/>
-      <c r="AB3" s="741"/>
-      <c r="AC3" s="741"/>
-      <c r="AD3" s="741"/>
-      <c r="AE3" s="741"/>
-      <c r="AF3" s="741"/>
-      <c r="AG3" s="741"/>
+      <c r="A3" s="743"/>
+      <c r="B3" s="740"/>
+      <c r="C3" s="740"/>
+      <c r="D3" s="740"/>
+      <c r="E3" s="740"/>
+      <c r="F3" s="740"/>
+      <c r="G3" s="740"/>
+      <c r="H3" s="740"/>
+      <c r="I3" s="740"/>
+      <c r="J3" s="740"/>
+      <c r="K3" s="740"/>
+      <c r="L3" s="740"/>
+      <c r="M3" s="740"/>
+      <c r="N3" s="740"/>
+      <c r="O3" s="740"/>
+      <c r="P3" s="740"/>
+      <c r="Q3" s="740"/>
+      <c r="R3" s="740"/>
+      <c r="S3" s="740"/>
+      <c r="T3" s="740"/>
+      <c r="U3" s="740"/>
+      <c r="V3" s="740"/>
+      <c r="W3" s="740"/>
+      <c r="X3" s="740"/>
+      <c r="Y3" s="740"/>
+      <c r="Z3" s="740"/>
+      <c r="AA3" s="740"/>
+      <c r="AB3" s="740"/>
+      <c r="AC3" s="740"/>
+      <c r="AD3" s="740"/>
+      <c r="AE3" s="740"/>
+      <c r="AF3" s="740"/>
+      <c r="AG3" s="740"/>
     </row>
     <row r="4" spans="1:99" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="735" t="s">
+      <c r="B4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="737" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="735" t="s">
+      <c r="G4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="737" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="735" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" s="735" t="s">
-        <v>13</v>
-      </c>
-      <c r="S4" s="735" t="s">
+      <c r="J4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" s="737" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" s="737" t="s">
         <v>13</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>1403</v>
       </c>
-      <c r="U4" s="735" t="s">
+      <c r="U4" s="737" t="s">
         <v>13</v>
       </c>
       <c r="V4" s="22" t="s">
@@ -7234,7 +7238,7 @@
         <v>13</v>
       </c>
       <c r="AE4" s="3">
-        <v>100</v>
+        <v>2400</v>
       </c>
       <c r="AF4" s="4" t="s">
         <v>1404</v>
@@ -18907,7 +18911,7 @@
       <c r="A153" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="B153" s="745"/>
+      <c r="B153" s="738"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
@@ -18966,7 +18970,7 @@
       <c r="A154" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="B154" s="745"/>
+      <c r="B154" s="738"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
@@ -19025,7 +19029,7 @@
       <c r="A155" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="B155" s="745"/>
+      <c r="B155" s="738"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
@@ -19084,7 +19088,7 @@
       <c r="A156" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="B156" s="745"/>
+      <c r="B156" s="738"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
@@ -19143,7 +19147,7 @@
       <c r="A157" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="B157" s="745"/>
+      <c r="B157" s="738"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
@@ -19202,7 +19206,7 @@
       <c r="A158" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="B158" s="745"/>
+      <c r="B158" s="738"/>
       <c r="C158" s="242" t="s">
         <v>13</v>
       </c>
@@ -19297,7 +19301,7 @@
       <c r="A159" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="B159" s="745"/>
+      <c r="B159" s="738"/>
       <c r="C159" s="241" t="s">
         <v>13</v>
       </c>
@@ -19392,7 +19396,7 @@
       <c r="A160" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="B160" s="745"/>
+      <c r="B160" s="738"/>
       <c r="C160" s="240" t="s">
         <v>13</v>
       </c>
@@ -19487,7 +19491,7 @@
       <c r="A161" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="B161" s="745"/>
+      <c r="B161" s="738"/>
       <c r="C161" s="239" t="s">
         <v>13</v>
       </c>
@@ -19582,7 +19586,7 @@
       <c r="A162" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="B162" s="745"/>
+      <c r="B162" s="738"/>
       <c r="C162" s="238" t="s">
         <v>13</v>
       </c>
@@ -52608,25 +52612,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B153:B162"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="N2:N3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="V2:V3"/>
@@ -52643,6 +52628,25 @@
     <mergeCell ref="AG2:AG3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B153:B162"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>